<commit_message>
Section Hero and Projects completed
</commit_message>
<xml_diff>
--- a/src/public/Documents/Personal Website US.xlsx
+++ b/src/public/Documents/Personal Website US.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Personal Project\our-page\src\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Personal Project\family-hub\src\public\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D79021-A8DD-4E02-A07B-FAAE1614770D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1D15D5-6F0C-4592-94C8-624541FDAA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" activeTab="1" xr2:uid="{EF2D9AA8-B161-44AD-8CC7-6192EAE41EB6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="86">
   <si>
     <t>Admin</t>
   </si>
@@ -165,9 +165,6 @@
     <t>to</t>
   </si>
   <si>
-    <t>12/2024</t>
-  </si>
-  <si>
     <t>10/2019</t>
   </si>
   <si>
@@ -280,6 +277,24 @@
   </si>
   <si>
     <t>COMSC 077</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Intern</t>
+  </si>
+  <si>
+    <t>2/2025</t>
+  </si>
+  <si>
+    <t>Branch Operations Officer</t>
+  </si>
+  <si>
+    <t>Relationship Banker</t>
+  </si>
+  <si>
+    <t>INSERT INTO works_at VALUES</t>
   </si>
 </sst>
 </file>
@@ -730,10 +745,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0737B84-FAAC-4674-AFD5-73AFA381037B}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -877,12 +892,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -895,57 +910,84 @@
       <c r="D19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>81</v>
+      </c>
+      <c r="I20" t="str">
+        <f>"("&amp;A20&amp;", "&amp;B20&amp;", '"&amp;C20&amp;"', '"&amp;D20&amp;"', '"&amp;E20&amp;"'),"</f>
+        <v>(1, 3, '5/2024', 'Current', 'Intern'),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" ref="I21:I22" si="0">"("&amp;A21&amp;", "&amp;B21&amp;", '"&amp;C21&amp;"', '"&amp;D21&amp;"', '"&amp;E21&amp;"'),"</f>
+        <v>(1, 1, '10/2019', '2/2025', 'Branch Operations Officer'),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>1</v>
-      </c>
-      <c r="B22">
-        <v>3</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>84</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="0"/>
+        <v>(1, 2, '1/2018', '9/2019', 'Relationship Banker'),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>49</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
@@ -960,7 +1002,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1</v>
       </c>
@@ -977,12 +1019,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
         <v>34</v>
@@ -996,12 +1038,12 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
         <v>29</v>
@@ -1012,7 +1054,7 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1020,7 +1062,7 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1028,7 +1070,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1036,12 +1078,12 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1049,16 +1091,16 @@
         <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" t="s">
+        <v>57</v>
+      </c>
+      <c r="D47" t="s">
         <v>58</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>59</v>
-      </c>
-      <c r="E47" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1072,7 +1114,7 @@
         <v>2</v>
       </c>
       <c r="D48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E48">
         <v>3.91</v>
@@ -1089,7 +1131,7 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E49">
         <v>3.9</v>
@@ -1097,18 +1139,18 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B53" t="s">
         <v>29</v>
       </c>
       <c r="C53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -1116,10 +1158,10 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
+        <v>65</v>
+      </c>
+      <c r="C54" t="s">
         <v>66</v>
-      </c>
-      <c r="C54" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -1127,10 +1169,10 @@
         <v>2</v>
       </c>
       <c r="B55" t="s">
+        <v>67</v>
+      </c>
+      <c r="C55" t="s">
         <v>68</v>
-      </c>
-      <c r="C55" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -1138,10 +1180,10 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" t="s">
         <v>70</v>
-      </c>
-      <c r="C56" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -1149,10 +1191,10 @@
         <v>4</v>
       </c>
       <c r="B57" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" t="s">
         <v>72</v>
-      </c>
-      <c r="C57" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -1160,10 +1202,10 @@
         <v>5</v>
       </c>
       <c r="B58" t="s">
+        <v>73</v>
+      </c>
+      <c r="C58" t="s">
         <v>74</v>
-      </c>
-      <c r="C58" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -1171,10 +1213,10 @@
         <v>6</v>
       </c>
       <c r="B59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -1182,10 +1224,10 @@
         <v>7</v>
       </c>
       <c r="B60" t="s">
+        <v>76</v>
+      </c>
+      <c r="C60" t="s">
         <v>77</v>
-      </c>
-      <c r="C60" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -1193,10 +1235,10 @@
         <v>8</v>
       </c>
       <c r="B61" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" t="s">
         <v>79</v>
-      </c>
-      <c r="C61" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1205,5 +1247,6 @@
     <hyperlink ref="F3" r:id="rId2" xr:uid="{9218B119-AB08-484F-94D2-1DA9A4F66639}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>